<commit_message>
ported over kroger api
</commit_message>
<xml_diff>
--- a/apps/api/src/data/RecipeSheet.xlsx
+++ b/apps/api/src/data/RecipeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gogura/cs5614/smartshelf/apps/api/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0DB821BB-A3FD-D84D-922F-3460B0F3C0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B5B7516F-FD24-3346-B91B-B811158B8BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{5710613C-42EE-7646-BA3B-6DD50F755840}"/>
+    <workbookView xWindow="7680" yWindow="3700" windowWidth="35840" windowHeight="21900" xr2:uid="{5710613C-42EE-7646-BA3B-6DD50F755840}"/>
   </bookViews>
   <sheets>
     <sheet name="RecipeSheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="239">
   <si>
     <t>name</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>chicken breast</t>
-  </si>
-  <si>
-    <t>eg</t>
   </si>
   <si>
     <t>beansprouts</t>
@@ -1211,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C844238B-F7D1-6143-8024-197930FE4168}">
   <dimension ref="A1:E341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1515,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1769,7 +1766,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -2054,7 +2051,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B49" t="str">
         <f>PROPER(A49)</f>
@@ -2381,7 +2378,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68" t="str">
         <f>PROPER(A68)</f>
@@ -2469,7 +2466,7 @@
         <v>0.5</v>
       </c>
       <c r="D73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E73">
         <v>7</v>
@@ -2669,11 +2666,11 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="B85" t="str">
         <f>PROPER(A85)</f>
-        <v>Eg</v>
+        <v>Egg</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -2684,7 +2681,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B86" t="str">
         <f>PROPER(A86)</f>
@@ -2702,7 +2699,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B87" t="str">
         <f>PROPER(A87)</f>
@@ -2720,7 +2717,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B88" t="str">
         <f>PROPER(A88)</f>
@@ -2738,7 +2735,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B89" t="str">
         <f>PROPER(A89)</f>
@@ -2774,7 +2771,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B91" t="str">
         <f>PROPER(A91)</f>
@@ -2792,7 +2789,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B92" t="str">
         <f>PROPER(A92)</f>
@@ -2828,7 +2825,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B94" t="str">
         <f>PROPER(A94)</f>
@@ -2846,7 +2843,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B95" t="str">
         <f>PROPER(A95)</f>
@@ -2864,7 +2861,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B96" t="str">
         <f>PROPER(A96)</f>
@@ -2900,7 +2897,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98" t="str">
         <f>PROPER(A98)</f>
@@ -2933,7 +2930,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B100" t="str">
         <f>PROPER(A100)</f>
@@ -2951,7 +2948,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B101" t="str">
         <f>PROPER(A101)</f>
@@ -2969,7 +2966,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B102" t="str">
         <f>PROPER(A102)</f>
@@ -2987,7 +2984,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B103" t="str">
         <f>PROPER(A103)</f>
@@ -3005,7 +3002,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" t="str">
         <f>PROPER(A104)</f>
@@ -3023,7 +3020,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B105" t="str">
         <f>PROPER(A105)</f>
@@ -3035,7 +3032,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B106" t="str">
         <f>PROPER(A106)</f>
@@ -3045,7 +3042,7 @@
         <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E106">
         <v>11</v>
@@ -3053,7 +3050,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B107" t="str">
         <f>PROPER(A107)</f>
@@ -3071,7 +3068,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B108" t="str">
         <f>PROPER(A108)</f>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B109" t="str">
         <f>PROPER(A109)</f>
@@ -3122,7 +3119,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B111" t="str">
         <f>PROPER(A111)</f>
@@ -3140,7 +3137,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B112" t="str">
         <f>PROPER(A112)</f>
@@ -3176,7 +3173,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="str">
         <f>PROPER(A114)</f>
@@ -3227,7 +3224,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B117" t="str">
         <f>PROPER(A117)</f>
@@ -3281,7 +3278,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120" t="str">
         <f>PROPER(A120)</f>
@@ -3299,7 +3296,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B121" t="str">
         <f>PROPER(A121)</f>
@@ -3309,7 +3306,7 @@
         <v>16</v>
       </c>
       <c r="D121" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E121">
         <v>13</v>
@@ -3317,7 +3314,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B122" t="str">
         <f>PROPER(A122)</f>
@@ -3335,7 +3332,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B123" t="str">
         <f>PROPER(A123)</f>
@@ -3353,7 +3350,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B124" t="str">
         <f>PROPER(A124)</f>
@@ -3368,7 +3365,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" t="str">
         <f>PROPER(A125)</f>
@@ -3398,7 +3395,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127" t="str">
         <f>PROPER(A127)</f>
@@ -3449,7 +3446,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B130" t="str">
         <f>PROPER(A130)</f>
@@ -3531,7 +3528,7 @@
         <v>0.5</v>
       </c>
       <c r="D134" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E134">
         <v>14</v>
@@ -3593,7 +3590,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B138" t="str">
         <f>PROPER(A138)</f>
@@ -3611,7 +3608,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B139" t="str">
         <f>PROPER(A139)</f>
@@ -3629,7 +3626,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B140" t="str">
         <f>PROPER(A140)</f>
@@ -3647,7 +3644,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B141" t="str">
         <f>PROPER(A141)</f>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B142" t="str">
         <f>PROPER(A142)</f>
@@ -3683,7 +3680,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B143" t="str">
         <f>PROPER(A143)</f>
@@ -3698,7 +3695,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B144" t="str">
         <f>PROPER(A144)</f>
@@ -3716,7 +3713,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B145" t="str">
         <f>PROPER(A145)</f>
@@ -3734,7 +3731,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B146" t="str">
         <f>PROPER(A146)</f>
@@ -3752,7 +3749,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B147" t="str">
         <f>PROPER(A147)</f>
@@ -3824,7 +3821,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B151" t="str">
         <f>PROPER(A151)</f>
@@ -3860,7 +3857,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B153" t="str">
         <f>PROPER(A153)</f>
@@ -3932,7 +3929,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B157" t="str">
         <f>PROPER(A157)</f>
@@ -3986,7 +3983,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B160" t="str">
         <f>PROPER(A160)</f>
@@ -4022,7 +4019,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B162" t="str">
         <f>PROPER(A162)</f>
@@ -4040,7 +4037,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B163" t="str">
         <f>PROPER(A163)</f>
@@ -4058,7 +4055,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B164" t="str">
         <f>PROPER(A164)</f>
@@ -4068,7 +4065,7 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E164">
         <v>16</v>
@@ -4076,7 +4073,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B165" t="str">
         <f>PROPER(A165)</f>
@@ -4094,7 +4091,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B166" t="str">
         <f>PROPER(A166)</f>
@@ -4163,7 +4160,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B170" t="str">
         <f>PROPER(A170)</f>
@@ -4173,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E170">
         <v>16</v>
@@ -4181,7 +4178,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B171" t="str">
         <f>PROPER(A171)</f>
@@ -4214,7 +4211,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B173" t="str">
         <f>PROPER(A173)</f>
@@ -4250,7 +4247,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B175" t="str">
         <f>PROPER(A175)</f>
@@ -4286,7 +4283,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B177" t="str">
         <f>PROPER(A177)</f>
@@ -4337,7 +4334,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B180" t="str">
         <f>PROPER(A180)</f>
@@ -4355,7 +4352,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B181" t="str">
         <f>PROPER(A181)</f>
@@ -4365,7 +4362,7 @@
         <v>0.75</v>
       </c>
       <c r="D181" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E181">
         <v>17</v>
@@ -4409,7 +4406,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" t="str">
         <f>PROPER(A184)</f>
@@ -4427,7 +4424,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B185" t="str">
         <f>PROPER(A185)</f>
@@ -4445,7 +4442,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B186" t="str">
         <f>PROPER(A186)</f>
@@ -4463,7 +4460,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B187" t="str">
         <f>PROPER(A187)</f>
@@ -4478,7 +4475,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B188" t="str">
         <f>PROPER(A188)</f>
@@ -4506,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="D189" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E189">
         <v>18</v>
@@ -4514,7 +4511,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B190" t="str">
         <f>PROPER(A190)</f>
@@ -4568,7 +4565,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B193" t="str">
         <f>PROPER(A193)</f>
@@ -4586,7 +4583,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B194" t="str">
         <f>PROPER(A194)</f>
@@ -4604,7 +4601,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B195" t="str">
         <f>PROPER(A195)</f>
@@ -4673,7 +4670,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B199" t="str">
         <f>PROPER(A199)</f>
@@ -4754,7 +4751,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B204" t="str">
         <f>PROPER(A204)</f>
@@ -4772,7 +4769,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B205" t="str">
         <f>PROPER(A205)</f>
@@ -4787,7 +4784,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B206" t="str">
         <f>PROPER(A206)</f>
@@ -4823,7 +4820,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B208" t="str">
         <f>PROPER(A208)</f>
@@ -4841,7 +4838,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B209" t="str">
         <f>PROPER(A209)</f>
@@ -4910,7 +4907,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B213" t="str">
         <f>PROPER(A213)</f>
@@ -4940,7 +4937,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B215" t="str">
         <f>PROPER(A215)</f>
@@ -4955,7 +4952,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B216" t="str">
         <f>PROPER(A216)</f>
@@ -4973,7 +4970,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B217" t="str">
         <f>PROPER(A217)</f>
@@ -4991,7 +4988,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B218" t="str">
         <f>PROPER(A218)</f>
@@ -5009,7 +5006,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B219" t="str">
         <f>PROPER(A219)</f>
@@ -5027,7 +5024,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B220" t="str">
         <f>PROPER(A220)</f>
@@ -5045,7 +5042,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B221" t="str">
         <f>PROPER(A221)</f>
@@ -5063,7 +5060,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B222" t="str">
         <f>PROPER(A222)</f>
@@ -5081,7 +5078,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B223" t="str">
         <f>PROPER(A223)</f>
@@ -5099,7 +5096,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B224" t="str">
         <f>PROPER(A224)</f>
@@ -5117,7 +5114,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B225" t="str">
         <f>PROPER(A225)</f>
@@ -5171,7 +5168,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B228" t="str">
         <f>PROPER(A228)</f>
@@ -5207,7 +5204,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B230" t="str">
         <f>PROPER(A230)</f>
@@ -5324,7 +5321,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B237" t="str">
         <f>PROPER(A237)</f>
@@ -5342,7 +5339,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B238" t="str">
         <f>PROPER(A238)</f>
@@ -5360,7 +5357,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B239" t="str">
         <f>PROPER(A239)</f>
@@ -5423,7 +5420,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B243" t="str">
         <f>PROPER(A243)</f>
@@ -5448,7 +5445,7 @@
         <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E244">
         <v>22</v>
@@ -5466,7 +5463,7 @@
         <v>1</v>
       </c>
       <c r="D245" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E245">
         <v>22</v>
@@ -5507,7 +5504,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B248" t="str">
         <f>PROPER(A248)</f>
@@ -5525,7 +5522,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B249" t="str">
         <f>PROPER(A249)</f>
@@ -5558,7 +5555,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B251" t="str">
         <f>PROPER(A251)</f>
@@ -5573,7 +5570,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B252" t="str">
         <f>PROPER(A252)</f>
@@ -5591,7 +5588,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B253" t="str">
         <f>PROPER(A253)</f>
@@ -5627,7 +5624,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B255" t="str">
         <f>PROPER(A255)</f>
@@ -5645,7 +5642,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B256" t="str">
         <f>PROPER(A256)</f>
@@ -5699,7 +5696,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B259" t="str">
         <f>PROPER(A259)</f>
@@ -5732,7 +5729,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B261" t="str">
         <f>PROPER(A261)</f>
@@ -5768,7 +5765,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B263" t="str">
         <f>PROPER(A263)</f>
@@ -5786,7 +5783,7 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B264" t="str">
         <f>PROPER(A264)</f>
@@ -5804,7 +5801,7 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B265" t="str">
         <f>PROPER(A265)</f>
@@ -5822,7 +5819,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B266" t="str">
         <f>PROPER(A266)</f>
@@ -5855,7 +5852,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B268" t="str">
         <f>PROPER(A268)</f>
@@ -5870,7 +5867,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B269" t="str">
         <f>PROPER(A269)</f>
@@ -5888,7 +5885,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B270" t="str">
         <f>PROPER(A270)</f>
@@ -6026,7 +6023,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B278" t="str">
         <f>PROPER(A278)</f>
@@ -6044,7 +6041,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B279" t="str">
         <f>PROPER(A279)</f>
@@ -6077,7 +6074,7 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B281" t="str">
         <f>PROPER(A281)</f>
@@ -6095,7 +6092,7 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B282" t="str">
         <f>PROPER(A282)</f>
@@ -6149,7 +6146,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B285" t="str">
         <f>PROPER(A285)</f>
@@ -6164,7 +6161,7 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B286" t="str">
         <f>PROPER(A286)</f>
@@ -6200,7 +6197,7 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B288" t="str">
         <f>PROPER(A288)</f>
@@ -6218,7 +6215,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B289" t="str">
         <f>PROPER(A289)</f>
@@ -6287,7 +6284,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B293" t="str">
         <f>PROPER(A293)</f>
@@ -6305,7 +6302,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B294" t="str">
         <f>PROPER(A294)</f>
@@ -6410,7 +6407,7 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B300" t="str">
         <f>PROPER(A300)</f>
@@ -6428,7 +6425,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B301" t="str">
         <f>PROPER(A301)</f>
@@ -6443,7 +6440,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B302" t="str">
         <f>PROPER(A302)</f>
@@ -6461,7 +6458,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B303" t="str">
         <f>PROPER(A303)</f>
@@ -6479,7 +6476,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B304" t="str">
         <f>PROPER(A304)</f>
@@ -6566,7 +6563,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B309" t="str">
         <f>PROPER(A309)</f>
@@ -6584,7 +6581,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B310" t="str">
         <f>PROPER(A310)</f>
@@ -6602,7 +6599,7 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B311" t="str">
         <f>PROPER(A311)</f>
@@ -6620,7 +6617,7 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B312" t="str">
         <f>PROPER(A312)</f>
@@ -6638,7 +6635,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B313" t="str">
         <f>PROPER(A313)</f>
@@ -6692,7 +6689,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B316" t="str">
         <f>PROPER(A316)</f>
@@ -6710,7 +6707,7 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B317" t="str">
         <f>PROPER(A317)</f>
@@ -6764,7 +6761,7 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B320" t="str">
         <f>PROPER(A320)</f>
@@ -6782,7 +6779,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B321" t="str">
         <f>PROPER(A321)</f>
@@ -6800,7 +6797,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B322" t="str">
         <f>PROPER(A322)</f>
@@ -6818,7 +6815,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B323" t="str">
         <f>PROPER(A323)</f>
@@ -6836,7 +6833,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B324" t="str">
         <f>PROPER(A324)</f>
@@ -6854,7 +6851,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B325" t="str">
         <f>PROPER(A325)</f>
@@ -6872,7 +6869,7 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B326" t="str">
         <f>PROPER(A326)</f>
@@ -6890,7 +6887,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B327" t="str">
         <f>PROPER(A327)</f>
@@ -6908,7 +6905,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B328" t="str">
         <f>PROPER(A328)</f>
@@ -6944,7 +6941,7 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B330" t="str">
         <f>PROPER(A330)</f>
@@ -6959,7 +6956,7 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B331" t="str">
         <f>PROPER(A331)</f>
@@ -7046,7 +7043,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B336" t="str">
         <f>PROPER(A336)</f>
@@ -7064,7 +7061,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B337" t="str">
         <f>PROPER(A337)</f>
@@ -7100,7 +7097,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B339" t="str">
         <f>PROPER(A339)</f>
@@ -7136,7 +7133,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B341" t="str">
         <f>PROPER(A341)</f>
@@ -7267,178 +7264,178 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>234</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>